<commit_message>
uploaded phylogenetic tree plots
</commit_message>
<xml_diff>
--- a/2nd_batch_analysis.xlsx
+++ b/2nd_batch_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flavi\Desktop\Tirocinio\Master-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE45F8B8-B128-45A6-BDDB-958C32CC0FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAD3114-74CC-4AFC-935E-9E52F7F4A17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-156" yWindow="192" windowWidth="12396" windowHeight="12048" activeTab="2" xr2:uid="{AA670B66-5D86-4ED2-AC4F-1FE3F6F5EE2E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AA670B66-5D86-4ED2-AC4F-1FE3F6F5EE2E}"/>
   </bookViews>
   <sheets>
     <sheet name="demulti" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="428">
   <si>
     <t>process_radtags v2.68, executed 2025-04-15 17:36:24 (zlib-1.3.1)</t>
   </si>
@@ -1310,6 +1310,16 @@
   </si>
   <si>
     <t>filtrato: populations -V populations.snps.chiara.recode.vcf -O filtrati/ -M populations2.txt --vcf  --write-random-snp --fstats --hwe --structure -t 32</t>
+  </si>
+  <si>
+    <t>ustacks --in-type gzfastq --file 03_filter/ALP1_clean_fastp.1.fq.gz --out-path 04_denovo -m 4 --name ALP1_clean_fastp -M 4  --force-diff-len --threads 80</t>
+  </si>
+  <si>
+    <t>/data/g_lambertini/lambertinic/miniconda3/envs/stacks/bin/denovo_map.pl --samples 03_filter/ --popmap ./populations2.txt --out-path 04_denovo/ --paired -m 4 -M 4 -n 1 -X ustacks: --force-diff-len -X populations: --vcf --threads 80 --min-samples-per-pop 0.80
+/data/g_lambertini/lambertinic/miniconda3/envs/stacks/bin/denovo_map.pl --samples 03_filter/ --popmap ./populations2.txt --out-path 04_denovo/ --paired -m 4 -M 4 -n 1 -X ustacks: --force-diff-len -X populations: --vcf --threads 80 --min-samples-per-pop 0.80</t>
+  </si>
+  <si>
+    <t>cstacks -n 1 --threads 80 -M ./populations2.txt -P 04_denovo</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1834,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1846,6 +1856,12 @@
     <xf numFmtId="9" fontId="0" fillId="35" borderId="0" xfId="43" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Colore 1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -9500,10 +9516,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B767BA-390E-48B9-884A-9A124631A8A6}">
-  <dimension ref="A1:K120"/>
+  <dimension ref="A1:AB120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="H1" sqref="H1:AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9517,7 +9533,7 @@
     <col min="11" max="12" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>295</v>
       </c>
@@ -9536,11 +9552,31 @@
       <c r="F1" t="s">
         <v>300</v>
       </c>
-      <c r="H1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>404</v>
       </c>
@@ -9560,10 +9596,10 @@
         <v>308</v>
       </c>
       <c r="H2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>401</v>
       </c>
@@ -9583,10 +9619,10 @@
         <v>304</v>
       </c>
       <c r="H3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -9606,10 +9642,10 @@
         <v>303</v>
       </c>
       <c r="H4" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -9629,10 +9665,10 @@
         <v>317</v>
       </c>
       <c r="H5" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -9652,10 +9688,10 @@
         <v>318</v>
       </c>
       <c r="H6" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>400</v>
       </c>
@@ -9675,10 +9711,10 @@
         <v>302</v>
       </c>
       <c r="H7" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>405</v>
       </c>
@@ -9698,10 +9734,10 @@
         <v>316</v>
       </c>
       <c r="H8" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>402</v>
       </c>
@@ -9721,10 +9757,10 @@
         <v>305</v>
       </c>
       <c r="H9" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>408</v>
       </c>
@@ -9744,10 +9780,10 @@
         <v>393</v>
       </c>
       <c r="H10" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>406</v>
       </c>
@@ -9766,8 +9802,11 @@
       <c r="F11" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>407</v>
       </c>
@@ -9786,8 +9825,11 @@
       <c r="F12" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>403</v>
       </c>
@@ -9807,14 +9849,10 @@
         <v>306</v>
       </c>
       <c r="H13" t="s">
-        <v>397</v>
-      </c>
-      <c r="I13" s="3">
-        <f>AVERAGE(C2:C104)</f>
-        <v>16.309417475728146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -9833,15 +9871,8 @@
       <c r="F14" t="s">
         <v>360</v>
       </c>
-      <c r="H14" t="s">
-        <v>398</v>
-      </c>
-      <c r="I14" s="3">
-        <f>STDEV(C2:C104)</f>
-        <v>4.3720163664285643</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -9860,15 +9891,8 @@
       <c r="F15" t="s">
         <v>354</v>
       </c>
-      <c r="H15" t="s">
-        <v>395</v>
-      </c>
-      <c r="I15" s="16">
-        <f>MIN(C2:C104)</f>
-        <v>8.94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -9886,13 +9910,6 @@
       </c>
       <c r="F16" t="s">
         <v>376</v>
-      </c>
-      <c r="H16" t="s">
-        <v>396</v>
-      </c>
-      <c r="I16" s="16">
-        <f>MAX(C2:C104)</f>
-        <v>41.09</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -9914,13 +9931,6 @@
       <c r="F17" t="s">
         <v>389</v>
       </c>
-      <c r="H17" t="s">
-        <v>399</v>
-      </c>
-      <c r="I17" s="16">
-        <f>MEDIAN(C2:C104)</f>
-        <v>15.71</v>
-      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -10001,6 +10011,13 @@
       <c r="F21" t="s">
         <v>328</v>
       </c>
+      <c r="H21" t="s">
+        <v>397</v>
+      </c>
+      <c r="I21" s="3">
+        <f>AVERAGE(C2:C104)</f>
+        <v>16.309417475728146</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -10021,6 +10038,13 @@
       <c r="F22" t="s">
         <v>350</v>
       </c>
+      <c r="H22" t="s">
+        <v>398</v>
+      </c>
+      <c r="I22" s="3">
+        <f>STDEV(C2:C104)</f>
+        <v>4.3720163664285643</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -10041,6 +10065,13 @@
       <c r="F23" t="s">
         <v>335</v>
       </c>
+      <c r="H23" t="s">
+        <v>395</v>
+      </c>
+      <c r="I23" s="16">
+        <f>MIN(C2:C104)</f>
+        <v>8.94</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -10061,6 +10092,13 @@
       <c r="F24" t="s">
         <v>363</v>
       </c>
+      <c r="H24" t="s">
+        <v>396</v>
+      </c>
+      <c r="I24" s="16">
+        <f>MAX(C2:C104)</f>
+        <v>41.09</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -10081,6 +10119,13 @@
       <c r="F25" t="s">
         <v>348</v>
       </c>
+      <c r="H25" t="s">
+        <v>399</v>
+      </c>
+      <c r="I25" s="16">
+        <f>MEDIAN(C2:C104)</f>
+        <v>15.71</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -11684,6 +11729,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:AB1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>